<commit_message>
Update notes on next steps
</commit_message>
<xml_diff>
--- a/yft_next_steps.xlsx
+++ b/yft_next_steps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ofp-sam\2023-assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{495ED1A8-52AC-4009-8874-E4013CE355BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5A0B0C-AC18-4126-8FBD-6F67B06CF3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{84E8502F-B80B-41CF-BFD9-DFAB7D3B00C8}"/>
+    <workbookView xWindow="1440" yWindow="0" windowWidth="14440" windowHeight="10340" xr2:uid="{84E8502F-B80B-41CF-BFD9-DFAB7D3B00C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Fix Shiny</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>Regional structure</t>
+  </si>
+  <si>
+    <t>new frq file from Thom 4 July 12:09</t>
+  </si>
+  <si>
+    <t>Explore Init</t>
+  </si>
+  <si>
+    <t>try changing only M or only K</t>
   </si>
 </sst>
 </file>
@@ -399,32 +408,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130040CC-0C5A-41F5-B214-67E7BE3735A8}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>